<commit_message>
Renamed scripts and updated readme file
</commit_message>
<xml_diff>
--- a/results/StreamMetabolism_LinearMixedEffect_output.xlsx
+++ b/results/StreamMetabolism_LinearMixedEffect_output.xlsx
@@ -413,19 +413,19 @@
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.224540805599668</v>
+        <v>-0.22454080560074</v>
       </c>
       <c r="D2" t="n">
-        <v>0.441750771254609</v>
+        <v>0.441750771261562</v>
       </c>
       <c r="E2" t="n">
-        <v>3.67397636623196</v>
+        <v>3.67397636613927</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.508297484035971</v>
+        <v>-0.508297484030398</v>
       </c>
       <c r="G2" t="n">
-        <v>0.640230080436361</v>
+        <v>0.640230080440596</v>
       </c>
     </row>
     <row r="3">
@@ -436,19 +436,19 @@
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>0.587205070131904</v>
+        <v>0.587205070131756</v>
       </c>
       <c r="D3" t="n">
-        <v>0.765404131938209</v>
+        <v>0.765404131950268</v>
       </c>
       <c r="E3" t="n">
-        <v>3.66878044462174</v>
+        <v>3.66878044407651</v>
       </c>
       <c r="F3" t="n">
-        <v>0.767183041780742</v>
+        <v>0.767183041768463</v>
       </c>
       <c r="G3" t="n">
-        <v>0.489350662423094</v>
+        <v>0.489350662435988</v>
       </c>
     </row>
     <row r="4">
@@ -459,19 +459,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.811896975700885</v>
+        <v>0.811896975700776</v>
       </c>
       <c r="D4" t="n">
-        <v>0.32749098924979</v>
+        <v>0.327490989252534</v>
       </c>
       <c r="E4" t="n">
-        <v>3.93747227954675</v>
+        <v>3.93747228301738</v>
       </c>
       <c r="F4" t="n">
-        <v>2.47914294546169</v>
+        <v>2.47914294544058</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0692680585712688</v>
+        <v>0.0692680585167203</v>
       </c>
     </row>
     <row r="5">
@@ -482,19 +482,19 @@
         <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>0.176043825757623</v>
+        <v>0.176043825757758</v>
       </c>
       <c r="D5" t="n">
-        <v>0.567335753755286</v>
+        <v>0.567335753760044</v>
       </c>
       <c r="E5" t="n">
-        <v>3.93993680529901</v>
+        <v>3.93993680799901</v>
       </c>
       <c r="F5" t="n">
-        <v>0.310299191602787</v>
+        <v>0.310299191600423</v>
       </c>
       <c r="G5" t="n">
-        <v>0.772053168625129</v>
+        <v>0.772053168616572</v>
       </c>
     </row>
     <row r="6">
@@ -505,19 +505,19 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>-2.56263122255275</v>
+        <v>-2.56263122255265</v>
       </c>
       <c r="D6" t="n">
-        <v>0.725406379436243</v>
+        <v>0.72540637943743</v>
       </c>
       <c r="E6" t="n">
-        <v>3.88781946158362</v>
+        <v>3.8878194576239</v>
       </c>
       <c r="F6" t="n">
-        <v>-3.5326836035607</v>
+        <v>-3.53268360355479</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0253317802527978</v>
+        <v>0.0253317802953824</v>
       </c>
     </row>
     <row r="7">
@@ -528,19 +528,19 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>0.596978384735906</v>
+        <v>0.596978384735661</v>
       </c>
       <c r="D7" t="n">
-        <v>1.25688586444343</v>
+        <v>1.2568858644455</v>
       </c>
       <c r="E7" t="n">
-        <v>3.89052164864578</v>
+        <v>3.89052164877885</v>
       </c>
       <c r="F7" t="n">
-        <v>0.474966265135185</v>
+        <v>0.474966265134211</v>
       </c>
       <c r="G7" t="n">
-        <v>0.660241696493821</v>
+        <v>0.660241696493634</v>
       </c>
     </row>
     <row r="8">
@@ -551,19 +551,19 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.02730824859318</v>
+        <v>-1.0273082485932</v>
       </c>
       <c r="D8" t="n">
-        <v>0.22992090559319</v>
+        <v>0.229920905594491</v>
       </c>
       <c r="E8" t="n">
-        <v>3.7951480835476</v>
+        <v>3.7951480840073</v>
       </c>
       <c r="F8" t="n">
-        <v>-4.46809412977367</v>
+        <v>-4.46809412974849</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0124941631793729</v>
+        <v>0.0124941631761959</v>
       </c>
     </row>
     <row r="9">
@@ -574,19 +574,19 @@
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>0.437891925484044</v>
+        <v>0.437891925483138</v>
       </c>
       <c r="D9" t="n">
-        <v>0.398016185701947</v>
+        <v>0.398016185704216</v>
       </c>
       <c r="E9" t="n">
-        <v>3.74803085317382</v>
+        <v>3.74803085398104</v>
       </c>
       <c r="F9" t="n">
-        <v>1.10018622662737</v>
+        <v>1.10018622661882</v>
       </c>
       <c r="G9" t="n">
-        <v>0.336842101775785</v>
+        <v>0.336842101766042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>